<commit_message>
modification il faut changer la matrice + MCD
</commit_message>
<xml_diff>
--- a/Dico données.xlsx
+++ b/Dico données.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L1dien\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22380" windowHeight="8808"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="78">
   <si>
     <t>ID_potion</t>
   </si>
@@ -248,10 +248,16 @@
     <t>ID_etat</t>
   </si>
   <si>
-    <t>Max 7</t>
-  </si>
-  <si>
     <t>#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEGRET </t>
+  </si>
+  <si>
+    <t>prix_recipient</t>
+  </si>
+  <si>
+    <t>numérique</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -375,12 +387,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -689,22 +731,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:B47"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -721,7 +763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -732,13 +774,13 @@
         <v>53</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -749,13 +791,13 @@
         <v>54</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -766,13 +808,13 @@
         <v>54</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -783,81 +825,81 @@
         <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -868,13 +910,13 @@
         <v>54</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -885,13 +927,13 @@
         <v>54</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -902,222 +944,218 @@
         <v>54</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="D16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B17" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="E24" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>56</v>
@@ -1129,377 +1167,394 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="D27" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="D28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="B29" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="D31" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="D32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="D33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="D34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B35" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="D35" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="D36" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="D37" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="D38" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B39" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="D39" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="D40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B41" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" s="4" t="s">
+      <c r="D41" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="B44" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="B46" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E46" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="B48" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E47" s="7" t="s">
+      <c r="D48" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>